<commit_message>
add decorators, fix market closed message
</commit_message>
<xml_diff>
--- a/analytics/industries/past-2-days-2021-03-15.xlsx
+++ b/analytics/industries/past-2-days-2021-03-15.xlsx
@@ -67,7 +67,7 @@
     <t xml:space="preserve">Gambling </t>
   </si>
   <si>
-    <t xml:space="preserve">Banks - Regional </t>
+    <t xml:space="preserve">Drug Manufacturers - Specialty Generic </t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -462,7 +462,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -470,7 +470,7 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2">

</xml_diff>

<commit_message>
update if/else to try/catch
</commit_message>
<xml_diff>
--- a/analytics/industries/past-2-days-2021-03-15.xlsx
+++ b/analytics/industries/past-2-days-2021-03-15.xlsx
@@ -40,15 +40,12 @@
     <t xml:space="preserve">Diagnostics Research </t>
   </si>
   <si>
+    <t xml:space="preserve">Internet Retail </t>
+  </si>
+  <si>
     <t xml:space="preserve">Biotechnology </t>
   </si>
   <si>
-    <t xml:space="preserve">Internet Retail </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Internet Content Information </t>
-  </si>
-  <si>
     <t xml:space="preserve">Telecom Services </t>
   </si>
   <si>
@@ -59,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">Exchange Traded Fund </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lodging </t>
   </si>
   <si>
     <t xml:space="preserve">Insurance - Property Casualty </t>
@@ -462,7 +462,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -478,7 +478,7 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -486,7 +486,7 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -510,7 +510,7 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">

</xml_diff>